<commit_message>
excel data confirmation may get error while sheet was copied, fixed manually.
</commit_message>
<xml_diff>
--- a/excel2db/modbus2db.xlsx
+++ b/excel2db/modbus2db.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20412"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhu\Desktop\PythonProject\EPICS\epics-programming\excel2db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2772C943-1E24-4720-9B6A-AE97B3D50B4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F15AFA8-9F69-4245-971A-DDFE89E12FC6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WorkArea" sheetId="5" r:id="rId1"/>
+    <sheet name="WorkArea" sheetId="6" r:id="rId1"/>
     <sheet name="example" sheetId="3" r:id="rId2"/>
     <sheet name="FormatSupported" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -27,11 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="161">
-  <si>
-    <t>Address(十进制)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="169">
   <si>
     <t>功能描述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -659,6 +655,37 @@
   <si>
     <t>——</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>处理周期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Address
+(十进制或十六进制)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x1235</t>
+  </si>
+  <si>
+    <t>0x1236</t>
+  </si>
+  <si>
+    <t>0x1237</t>
+  </si>
+  <si>
+    <t>0x1238</t>
+  </si>
+  <si>
+    <t>0x1239</t>
+  </si>
+  <si>
+    <t>0x1240</t>
   </si>
 </sst>
 </file>
@@ -730,7 +757,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1032,11 +1059,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1122,18 +1177,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1142,47 +1242,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1463,292 +1522,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C162B7E-186D-458D-B234-95F189D016FF}">
-  <dimension ref="A1:W8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:W1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="45" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.21875" style="45" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.77734375" style="45" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="45" customWidth="1"/>
-    <col min="9" max="9" width="35.109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.44140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" style="45" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.77734375" style="45" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" style="45" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.6640625" style="45" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.5546875" style="45" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.44140625" style="45" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="13" style="45" customWidth="1"/>
-    <col min="24" max="16384" width="8.88671875" style="45"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" s="3" customFormat="1" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="46"/>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="47"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="46"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="47"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="47"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="47"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="47"/>
-      <c r="L5" s="47"/>
-      <c r="M5" s="47"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="47"/>
-      <c r="R5" s="47"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
-      <c r="N6" s="47"/>
-      <c r="O6" s="47"/>
-      <c r="P6" s="47"/>
-      <c r="Q6" s="47"/>
-      <c r="R6" s="47"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
-      <c r="N7" s="47"/>
-      <c r="O7" s="47"/>
-      <c r="P7" s="47"/>
-      <c r="Q7" s="47"/>
-      <c r="R7" s="47"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
-      <c r="N8" s="47"/>
-      <c r="O8" s="47"/>
-      <c r="P8" s="47"/>
-      <c r="Q8" s="47"/>
-      <c r="R8" s="47"/>
-    </row>
-  </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="C2:C8"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3F827E8-A33E-4102-A948-FD7EEC466DA3}">
-          <x14:formula1>
-            <xm:f>FormatSupported!$D$3:$D$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{803FBDB2-0CC2-4125-9103-20E2C3A541E5}">
-          <x14:formula1>
-            <xm:f>FormatSupported!$B$3:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FBC16784-B055-48BB-BACF-871BE125C1DB}">
-          <x14:formula1>
-            <xm:f>FormatSupported!$H$3:$H$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>P2:Q1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21580DD4-068D-46EA-81C8-337E9E22FE69}">
-          <x14:formula1>
-            <xm:f>FormatSupported!$F$3:$F$14</xm:f>
-          </x14:formula1>
-          <xm:sqref>Q2:Q1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88599853-7CB8-4592-94C0-13EF1A342763}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B8A488-4CED-4A2D-9594-C2DD5F104F1E}">
   <dimension ref="A1:W15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -1756,7 +1534,7 @@
     <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.21875" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
@@ -1778,745 +1556,1171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="3" customFormat="1" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="C1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="30"/>
+      <c r="Q6" s="30"/>
+      <c r="R6" s="30"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="30"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="41"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="C2:C8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B42C24CD-215D-49D1-A6E0-2FA4087BD5DA}">
+          <x14:formula1>
+            <xm:f>FormatSupported!$N$3:$N$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BCFBF84B-9E23-4BA9-A437-8D5E87BCA264}">
+          <x14:formula1>
+            <xm:f>FormatSupported!$D$3:$D$16</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{51BACBAB-5D59-47F5-AE87-664E0D57216E}">
+          <x14:formula1>
+            <xm:f>FormatSupported!$B$3:$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1D0C4646-59E0-4A84-AA63-AB90AA357DAD}">
+          <x14:formula1>
+            <xm:f>FormatSupported!$H$3:$H$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2:P1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E035A380-772A-4B24-9781-8BF4FA156F6D}">
+          <x14:formula1>
+            <xm:f>FormatSupported!$F$3:$F$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q2:Q1048576 Q2:Q1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88599853-7CB8-4592-94C0-13EF1A342763}">
+  <dimension ref="A1:W15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="13" style="1" customWidth="1"/>
+    <col min="24" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="3" customFormat="1" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="C2" s="31"/>
+      <c r="B2" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="47"/>
       <c r="D2" s="9">
         <v>10000</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H2" s="27">
         <v>2</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="9">
         <v>3</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>53</v>
-      </c>
       <c r="R2" s="9"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="4">
-        <v>10000</v>
+      <c r="A3" s="46"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="38">
+        <v>10001</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H3" s="27">
         <v>2</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" s="4">
         <v>3</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="4">
-        <v>10000</v>
+      <c r="A4" s="46"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="38">
+        <v>10002</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H4" s="27">
         <v>2</v>
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="4">
         <v>3</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="4">
-        <v>10000</v>
+      <c r="A5" s="46"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="38">
+        <v>10003</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H5" s="27">
         <v>2</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N5" s="4">
         <v>3</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S5" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>133</v>
-      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="4">
-        <v>10000</v>
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="38">
+        <v>10004</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H6" s="27">
         <v>2</v>
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N6" s="4">
         <v>3</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="4">
-        <v>10000</v>
+      <c r="A7" s="46"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="38">
+        <v>10005</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H7" s="27">
         <v>2</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N7" s="4">
         <v>3</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="4">
-        <v>10000</v>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="38">
+        <v>10006</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H8" s="28">
         <v>4</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N8" s="4">
         <v>3</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="4">
-        <v>10000</v>
+      <c r="A9" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H9" s="28">
         <v>4</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N9" s="4">
         <v>3</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="4">
-        <v>10000</v>
+      <c r="A10" s="46"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="39" t="s">
+        <v>163</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H10" s="28">
         <v>8</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N10" s="4">
         <v>3</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="4">
-        <v>10000</v>
+      <c r="A11" s="46"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="39" t="s">
+        <v>164</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H11" s="28">
         <v>8</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="N11" s="4">
         <v>3</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="4">
-        <v>10000</v>
+      <c r="A12" s="46"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="39" t="s">
+        <v>165</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="28">
         <v>4</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N12" s="4">
         <v>3</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R12" s="4"/>
       <c r="S12" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="4">
-        <v>10000</v>
+      <c r="A13" s="46"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="39" t="s">
+        <v>166</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H13" s="28">
         <v>8</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N13" s="4">
         <v>3</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="R13" s="4"/>
       <c r="S13" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="4">
-        <v>10000</v>
+      <c r="A14" s="46"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="46"/>
+      <c r="D14" s="39" t="s">
+        <v>167</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="28">
         <v>10</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N14" s="4">
         <v>3</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="R14" s="4"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="4">
-        <v>10000</v>
+      <c r="A15" s="46"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="39" t="s">
+        <v>168</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H15" s="28">
         <v>10</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N15" s="4">
         <v>3</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R15" s="4"/>
     </row>
@@ -2536,7 +2740,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{93ABAE30-01B3-4072-86BD-646F06B3E7DF}">
           <x14:formula1>
             <xm:f>FormatSupported!$F$3:$F$14</xm:f>
@@ -2561,6 +2765,12 @@
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5C7A66C1-D8F8-425B-AB5C-F427DD08EEFF}">
+          <x14:formula1>
+            <xm:f>FormatSupported!$N$3:$N$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -2569,10 +2779,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CC9308-14F5-49E7-9EC1-96613602423E}">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -2588,328 +2798,362 @@
     <col min="9" max="9" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="13" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" s="2" customFormat="1" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" s="2" customFormat="1" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="19"/>
-      <c r="D2" s="42" t="s">
-        <v>159</v>
+      <c r="D2" s="37" t="s">
+        <v>158</v>
       </c>
       <c r="E2" s="19"/>
       <c r="F2" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="35"/>
-    </row>
-    <row r="3" spans="2:12" ht="17.399999999999999" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="50"/>
+      <c r="N2" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E3" s="20"/>
       <c r="F3" s="17"/>
       <c r="G3" s="21"/>
       <c r="H3" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="J3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="L3" s="27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="40"/>
+        <v>5</v>
+      </c>
+      <c r="C4" s="35"/>
       <c r="D4" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" s="41"/>
+        <v>66</v>
+      </c>
+      <c r="E4" s="36"/>
       <c r="F4" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I4" s="11"/>
-      <c r="J4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L4" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="21"/>
       <c r="D5" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5" s="21"/>
       <c r="F5" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="J5" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="K5" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="L5" s="27" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="L5" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D6" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="21"/>
       <c r="H6" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N6" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D7" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N7" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D8" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="21"/>
       <c r="H8" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L8" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N8" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D9" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N9" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D10" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L10" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N10" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="D11" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="N11" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="K13" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="L13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L13" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D15" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D15" s="14" t="s">
+    </row>
+    <row r="16" spans="2:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="I2:L2"/>
   </mergeCells>

</xml_diff>